<commit_message>
started making some quality assurance plans for UI which I have nearly finished
</commit_message>
<xml_diff>
--- a/COMP2160 Assignment 2/Assets/Documentation/QualityAssurancePlan.xlsx
+++ b/COMP2160 Assignment 2/Assets/Documentation/QualityAssurancePlan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\COMP1150\github\Assignment2\COMP2160 Assignment 2\Assets\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9446D020-3169-428F-8522-FC48DBD4CEA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA808376-D2F0-4D25-9323-C64698DE4698}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-35805" yWindow="3405" windowWidth="18990" windowHeight="15735" xr2:uid="{46A80917-E6E0-4F32-A602-42283E706FEA}"/>
+    <workbookView xWindow="564" yWindow="372" windowWidth="22476" windowHeight="16800" xr2:uid="{46A80917-E6E0-4F32-A602-42283E706FEA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t>Test ID</t>
   </si>
@@ -47,6 +47,36 @@
   </si>
   <si>
     <t>Test Scene</t>
+  </si>
+  <si>
+    <t>Sample Scene</t>
+  </si>
+  <si>
+    <t>Run the game in a 16:9 screen aspect ratio (on maximum play as well). 
+Observe any changes to the user interface across different screen sizes on a 16:9 aspect ratio.</t>
+  </si>
+  <si>
+    <t>The UI should not warp or alter on a 16:9 screen aspect ratio</t>
+  </si>
+  <si>
+    <t>Run the game in a 16:9 screen aspect ratio.
+Collide the player with different objects and observe the health bar's changes</t>
+  </si>
+  <si>
+    <t>The UI for the health bar at the top should indicate that the player is losing health (i.e. it starts out green at maximum health and shows more red as it loses health)</t>
+  </si>
+  <si>
+    <t>6(b)</t>
+  </si>
+  <si>
+    <t>Run the game in a 16:9 screen aspect ratio. 
+Observe the timer as it runs in real time from seconds to minutes of starting the game.</t>
+  </si>
+  <si>
+    <t>6(a)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The UI for the timer should be displayed in a real time '00:00:00' in minutes, seconds and milliseconds- in that order. The timer should keep </t>
   </si>
 </sst>
 </file>
@@ -102,7 +132,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
@@ -113,6 +143,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -432,16 +474,16 @@
   <dimension ref="A1:E40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="7.44140625" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.44140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5546875" style="4" customWidth="1"/>
+    <col min="4" max="4" width="44.88671875" style="8" customWidth="1"/>
+    <col min="5" max="5" width="51.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.35">
@@ -461,19 +503,55 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B2" s="4">
+        <v>6</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>3</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>